<commit_message>
Update Excel - Project -VS-Updated.xlsx
</commit_message>
<xml_diff>
--- a/Excel - Project -VS-Updated.xlsx
+++ b/Excel - Project -VS-Updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/176528a26ee13369/Documents/Goodwill/GitHub/Data-Analyst_Excel-Project_VS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1246" documentId="8_{624EE273-237A-4852-8522-D12196B3FB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{192CDDFC-D6EE-49BE-B626-A20165E91206}"/>
+  <xr:revisionPtr revIDLastSave="1313" documentId="8_{624EE273-237A-4852-8522-D12196B3FB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCD43D8D-AEE3-433D-9131-C2F9A2859C32}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="923" xr2:uid="{3F396370-2144-4D01-B693-F4E0D3CB5C02}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="158">
   <si>
     <t>Employee ID</t>
   </si>
@@ -1282,7 +1282,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1305,12 +1304,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
@@ -1330,11 +1323,20 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5904,8 +5906,8 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6441,8 +6443,9 @@
       <c r="E17" s="13">
         <v>50545</v>
       </c>
-      <c r="F17" s="71" t="s">
-        <v>151</v>
+      <c r="F17" s="71" t="str">
+        <f>_xlfn.XLOOKUP(EMPData[[#This Row],[Employee ID]],EmpBonus[Employee ID],EmpBonus[Bonus %],"-")</f>
+        <v>-</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>40</v>
@@ -6757,8 +6760,9 @@
       <c r="E27" s="13">
         <v>60270</v>
       </c>
-      <c r="F27" s="71" t="s">
-        <v>151</v>
+      <c r="F27" s="71" t="str">
+        <f>_xlfn.XLOOKUP(EMPData[[#This Row],[Employee ID]],EmpBonus[Employee ID],EmpBonus[Bonus %],"-")</f>
+        <v>-</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>23</v>
@@ -6786,7 +6790,7 @@
       <c r="E28" s="13">
         <v>60445</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="71">
         <f>EMPData[[#This Row],[Yearly Sal]]*_xlfn.XLOOKUP(EMPData[[#This Row],[Employee ID]],EmpBonus[Employee ID],EmpBonus[Bonus %])</f>
         <v>11484.55</v>
       </c>
@@ -6846,8 +6850,9 @@
       <c r="E30" s="13">
         <v>68357</v>
       </c>
-      <c r="F30" s="71" t="s">
-        <v>151</v>
+      <c r="F30" s="71" t="str">
+        <f>_xlfn.XLOOKUP(EMPData[[#This Row],[Employee ID]],EmpBonus[Employee ID],EmpBonus[Bonus %],"-")</f>
+        <v>-</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>71</v>
@@ -7055,8 +7060,9 @@
       <c r="E37" s="13">
         <v>88357</v>
       </c>
-      <c r="F37" s="71" t="s">
-        <v>151</v>
+      <c r="F37" s="71" t="str">
+        <f>_xlfn.XLOOKUP(EMPData[[#This Row],[Employee ID]],EmpBonus[Employee ID],EmpBonus[Bonus %],"-")</f>
+        <v>-</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>85</v>
@@ -7234,8 +7240,9 @@
       <c r="E43" s="13">
         <v>93668</v>
       </c>
-      <c r="F43" s="71" t="s">
-        <v>151</v>
+      <c r="F43" s="71" t="str">
+        <f>_xlfn.XLOOKUP(EMPData[[#This Row],[Employee ID]],EmpBonus[Employee ID],EmpBonus[Bonus %],"-")</f>
+        <v>-</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>97</v>
@@ -7510,6 +7517,9 @@
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F30 F27 F37 F17 F43" formula="1"/>
+  </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -7525,7 +7535,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J75"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7608,10 +7618,10 @@
       <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:18" ht="19" thickBot="1">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="73" t="s">
         <v>156</v>
       </c>
       <c r="I2" s="46">
@@ -8054,7 +8064,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8093,10 +8103,10 @@
       <c r="B2" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="90"/>
+      <c r="D2" s="98"/>
       <c r="H2" s="39">
         <v>1</v>
       </c>
@@ -8224,7 +8234,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8257,13 +8267,13 @@
       <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" ht="19" thickBot="1">
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="99" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="101"/>
+      <c r="E2" s="100"/>
       <c r="K2" s="39">
         <v>2</v>
       </c>
@@ -8272,14 +8282,14 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1">
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="99">
+      <c r="D3" s="96">
         <f>SUMIF(EMPData[Department],"sales",EMPData[Yearly Sal])</f>
         <v>1294801</v>
       </c>
-      <c r="E3" s="96">
+      <c r="E3" s="93">
         <f>D3</f>
         <v>1294801</v>
       </c>
@@ -8288,33 +8298,33 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="92">
         <f>SUMIF(EMPData[Department],"procurement",EMPData[Yearly Sal])</f>
         <v>1053666</v>
       </c>
-      <c r="E4" s="96">
+      <c r="E4" s="93">
         <f t="shared" ref="E4:E5" si="0">D4</f>
         <v>1053666</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1">
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="97">
+      <c r="D5" s="94">
         <f>SUMIF(EMPData[Department],"finance",EMPData[Yearly Sal])</f>
         <v>1271409</v>
       </c>
-      <c r="E5" s="98">
+      <c r="E5" s="95">
         <f t="shared" si="0"/>
         <v>1271409</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="L7" s="73"/>
+      <c r="L7" s="72"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
@@ -8372,7 +8382,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8534,7 +8544,7 @@
   <dimension ref="A1:P104"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I25"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9607,7 +9617,7 @@
       <c r="B2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="73" t="s">
         <v>155</v>
       </c>
       <c r="I2" s="46">
@@ -9655,7 +9665,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K44"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9695,19 +9705,19 @@
       <c r="B2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="83" t="s">
         <v>157</v>
       </c>
       <c r="H2" s="60" t="s">
@@ -9724,22 +9734,22 @@
       <c r="B3" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="79">
+      <c r="F3" s="78">
         <v>21971</v>
       </c>
-      <c r="G3" s="80">
+      <c r="G3" s="79">
         <v>0.23</v>
       </c>
-      <c r="H3" s="81">
+      <c r="H3" s="80">
         <f>Master!E4*_xlfn.XLOOKUP(Master!A4,Master!H4:H43,Master!I4:I43)</f>
         <v>5053.33</v>
       </c>
@@ -9764,6 +9774,7 @@
         <v>0.1</v>
       </c>
       <c r="H4" s="33">
+        <f>Master!E5*_xlfn.XLOOKUP(Master!A5,Master!H4:H43,Master!I4:I43)</f>
         <v>2972.6000000000004</v>
       </c>
       <c r="K4" t="s">
@@ -9790,6 +9801,7 @@
         <v>0.27</v>
       </c>
       <c r="H5" s="33">
+        <f>F5*_xlfn.XLOOKUP(B5,B3:B21,G3:G21)</f>
         <v>9398.16</v>
       </c>
     </row>
@@ -9813,6 +9825,7 @@
         <v>0.23</v>
       </c>
       <c r="H6" s="33">
+        <f>F6*_xlfn.XLOOKUP(B6,B3:B21,G3:G21)</f>
         <v>9114.2100000000009</v>
       </c>
       <c r="K6" t="s">
@@ -9839,6 +9852,7 @@
         <v>0.09</v>
       </c>
       <c r="H7" s="33">
+        <f>F7*_xlfn.XLOOKUP(B7,B3:B21,G3:G21)</f>
         <v>4050</v>
       </c>
     </row>
@@ -9862,6 +9876,7 @@
         <v>0.24</v>
       </c>
       <c r="H8" s="33">
+        <f>F8*_xlfn.XLOOKUP(B8,B3:B21,G3:G21)</f>
         <v>10828.08</v>
       </c>
     </row>
@@ -9885,10 +9900,11 @@
         <v>0.25</v>
       </c>
       <c r="H9" s="33">
+        <f>F9*_xlfn.XLOOKUP(B9,B3:B21,G3:G21)</f>
         <v>12636.25</v>
       </c>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="26" t="s">
@@ -9910,6 +9926,7 @@
         <v>0.13</v>
       </c>
       <c r="H10" s="33">
+        <f>F10*_xlfn.XLOOKUP(B10,B3:B21,G3:G21)</f>
         <v>7165.21</v>
       </c>
     </row>
@@ -9933,9 +9950,10 @@
         <v>0.22</v>
       </c>
       <c r="H11" s="33">
+        <f t="shared" ref="H6:H21" si="0">F11*_xlfn.XLOOKUP(B11,B9:B27,G9:G27)</f>
         <v>12857.9</v>
       </c>
-      <c r="L11" s="88"/>
+      <c r="L11" s="87"/>
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="26" t="s">
@@ -9957,9 +9975,10 @@
         <v>0.11</v>
       </c>
       <c r="H12" s="33">
+        <f>F12*_xlfn.XLOOKUP(B12,B3:B21,G3:G21)</f>
         <v>6428.95</v>
       </c>
-      <c r="L12" s="88"/>
+      <c r="L12" s="87"/>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="26" t="s">
@@ -9977,13 +9996,14 @@
       <c r="F13" s="31">
         <v>60270</v>
       </c>
-      <c r="G13" s="86" t="s">
+      <c r="G13" s="85" t="s">
         <v>151</v>
       </c>
-      <c r="H13" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="L13" s="88"/>
+      <c r="H13" s="101" t="str">
+        <f>_xlfn.XLOOKUP(B13,B3:B21,G3:G21,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="L13" s="87"/>
     </row>
     <row r="14" spans="1:14">
       <c r="B14" s="26" t="s">
@@ -10005,6 +10025,7 @@
         <v>0.19</v>
       </c>
       <c r="H14" s="33">
+        <f>F14*_xlfn.XLOOKUP(B14,B3:B21,G3:G21)</f>
         <v>11484.55</v>
       </c>
     </row>
@@ -10028,9 +10049,10 @@
         <v>0.06</v>
       </c>
       <c r="H15" s="33">
+        <f>F15*_xlfn.XLOOKUP(B15,B3:B21,G3:G21)</f>
         <v>4800</v>
       </c>
-      <c r="L15" s="88"/>
+      <c r="L15" s="87"/>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="26" t="s">
@@ -10052,6 +10074,7 @@
         <v>0.2</v>
       </c>
       <c r="H16" s="33">
+        <f>F16*_xlfn.XLOOKUP(B16,B3:B21,G3:G21)</f>
         <v>16623.400000000001</v>
       </c>
     </row>
@@ -10075,6 +10098,7 @@
         <v>0.06</v>
       </c>
       <c r="H17" s="33">
+        <f>F17*_xlfn.XLOOKUP(B17,B3:B21,G3:G21)</f>
         <v>5370</v>
       </c>
     </row>
@@ -10094,11 +10118,12 @@
       <c r="F18" s="31">
         <v>93668</v>
       </c>
-      <c r="G18" s="85" t="s">
+      <c r="G18" s="84" t="s">
         <v>151</v>
       </c>
-      <c r="H18" s="71" t="s">
-        <v>151</v>
+      <c r="H18" s="101" t="str">
+        <f>_xlfn.XLOOKUP(B18,B3:B21,G3:G21, "-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -10121,9 +10146,10 @@
         <v>0.13</v>
       </c>
       <c r="H19" s="33">
+        <f>F19*_xlfn.XLOOKUP(B19,B3:B21,G3:G21)</f>
         <v>15600</v>
       </c>
-      <c r="L19" s="88"/>
+      <c r="L19" s="87"/>
     </row>
     <row r="20" spans="1:12">
       <c r="B20" s="26" t="s">
@@ -10145,106 +10171,108 @@
         <v>0.08</v>
       </c>
       <c r="H20" s="33">
+        <f>F20*_xlfn.XLOOKUP(B20,B3:B21,G3:G21)</f>
         <v>10720</v>
       </c>
-      <c r="L20" s="88"/>
+      <c r="L20" s="87"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1">
       <c r="B21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="75" t="s">
+      <c r="D21" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="75" t="s">
+      <c r="E21" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="75">
         <v>135000</v>
       </c>
-      <c r="G21" s="77">
+      <c r="G21" s="76">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H21" s="72">
+      <c r="H21" s="33">
+        <f>F21*_xlfn.XLOOKUP(B21,B3:B21,G3:G21)</f>
         <v>18900</v>
       </c>
-      <c r="L21" s="88"/>
+      <c r="L21" s="87"/>
     </row>
     <row r="22" spans="1:12">
       <c r="F22" s="70"/>
       <c r="G22" s="70"/>
       <c r="H22" s="15"/>
-      <c r="L22" s="88"/>
+      <c r="L22" s="87"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>141</v>
       </c>
-      <c r="L23" s="88"/>
+      <c r="L23" s="87"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="L24" s="88"/>
+      <c r="L24" s="87"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="L25" s="88"/>
+      <c r="L25" s="87"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="L28" s="88"/>
+      <c r="L28" s="87"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="L29" s="88"/>
+      <c r="L29" s="87"/>
     </row>
     <row r="34" spans="12:12">
-      <c r="L34" s="88"/>
+      <c r="L34" s="87"/>
     </row>
     <row r="35" spans="12:12">
-      <c r="L35" s="88"/>
+      <c r="L35" s="87"/>
     </row>
     <row r="36" spans="12:12">
-      <c r="L36" s="88"/>
+      <c r="L36" s="87"/>
     </row>
     <row r="37" spans="12:12">
-      <c r="L37" s="88"/>
+      <c r="L37" s="87"/>
     </row>
     <row r="38" spans="12:12">
-      <c r="L38" s="88"/>
+      <c r="L38" s="87"/>
     </row>
     <row r="39" spans="12:12">
-      <c r="L39" s="88"/>
+      <c r="L39" s="87"/>
     </row>
     <row r="40" spans="12:12">
-      <c r="L40" s="88"/>
+      <c r="L40" s="87"/>
     </row>
     <row r="41" spans="12:12">
-      <c r="L41" s="88"/>
+      <c r="L41" s="87"/>
     </row>
     <row r="42" spans="12:12">
-      <c r="L42" s="88"/>
+      <c r="L42" s="87"/>
     </row>
     <row r="43" spans="12:12">
-      <c r="L43" s="88"/>
+      <c r="L43" s="87"/>
     </row>
     <row r="46" spans="12:12">
-      <c r="L46" s="88"/>
+      <c r="L46" s="87"/>
     </row>
     <row r="47" spans="12:12">
-      <c r="L47" s="88"/>
+      <c r="L47" s="87"/>
     </row>
     <row r="48" spans="12:12">
-      <c r="L48" s="88"/>
+      <c r="L48" s="87"/>
     </row>
     <row r="49" spans="12:12">
-      <c r="L49" s="88"/>
+      <c r="L49" s="87"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:H21" xr:uid="{A3A9DB0C-8F70-4F7C-A3D1-8A0F1AD171BC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H3" formulaRange="1"/>
+    <ignoredError sqref="H3:H4" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>